<commit_message>
Crypto bot created with SAC
</commit_message>
<xml_diff>
--- a/Notes/Table.xlsx
+++ b/Notes/Table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BLACKBOX\Desktop\RL New\tfrl-cookbook\Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B67E2388-CAFB-4849-A000-8F7C02A74A62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86C0DC7D-2BAB-4D78-AC23-19C5CE9C5CB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Algorithm</t>
   </si>
@@ -47,9 +47,6 @@
   </si>
   <si>
     <t>Matching Scenarios in General</t>
-  </si>
-  <si>
-    <t>Problems that can't be analyzed</t>
   </si>
   <si>
     <t>DQN</t>
@@ -129,6 +126,78 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>428625</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>68581</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>474344</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="TextBox 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1336B133-0F16-2257-C24C-409A642A5039}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9944100" y="3497581"/>
+          <a:ext cx="45719" cy="45719"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -389,10 +458,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -405,11 +474,10 @@
     <col min="6" max="6" width="15.28515625" customWidth="1"/>
     <col min="7" max="7" width="17.42578125" customWidth="1"/>
     <col min="8" max="8" width="18.140625" customWidth="1"/>
-    <col min="9" max="9" width="24.7109375" customWidth="1"/>
-    <col min="10" max="10" width="33.85546875" customWidth="1"/>
+    <col min="9" max="9" width="34.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -437,53 +505,51 @@
       <c r="I1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" t="s">
         <v>10</v>
       </c>
-      <c r="B2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3" t="s">
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
-      <c r="A4" t="s">
+    <row r="5" spans="1:9">
+      <c r="A5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
-      <c r="A5" t="s">
+    <row r="6" spans="1:9">
+      <c r="A6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
-      <c r="A6" t="s">
+    <row r="7" spans="1:9">
+      <c r="A7" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
-      <c r="A7" t="s">
+    <row r="8" spans="1:9">
+      <c r="A8" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
-      <c r="A8" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>